<commit_message>
working on general problem section
</commit_message>
<xml_diff>
--- a/Data/mpfamilies_structure.xlsx
+++ b/Data/mpfamilies_structure.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -281,12 +281,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -305,9 +311,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -591,8 +598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -640,7 +647,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B7" t="s">
@@ -648,7 +655,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B8" t="s">
@@ -656,7 +663,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B9" t="s">
@@ -664,7 +671,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B10" t="s">
@@ -802,7 +809,7 @@
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="A31" s="2" t="s">
         <v>49</v>
       </c>
     </row>
@@ -812,12 +819,12 @@
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="A33" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+      <c r="A34" s="2" t="s">
         <v>52</v>
       </c>
     </row>
@@ -827,7 +834,7 @@
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+      <c r="A36" s="2" t="s">
         <v>54</v>
       </c>
     </row>
@@ -871,7 +878,7 @@
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="A43" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B43" t="s">

</xml_diff>

<commit_message>
first draft of intro
</commit_message>
<xml_diff>
--- a/Data/mpfamilies_structure.xlsx
+++ b/Data/mpfamilies_structure.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="88">
   <si>
     <t>state</t>
   </si>
@@ -243,6 +244,54 @@
   </si>
   <si>
     <t>fips code of ssn issuing state</t>
+  </si>
+  <si>
+    <t>Matching Methods</t>
+  </si>
+  <si>
+    <t>Estimation Methods</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deterministic </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Probababilistic </t>
+  </si>
+  <si>
+    <t>No match weights</t>
+  </si>
+  <si>
+    <t>Uses match weights</t>
+  </si>
+  <si>
+    <t>ABE (2012,2014,2017)</t>
+  </si>
+  <si>
+    <t>Aizer et al. (2016)</t>
+  </si>
+  <si>
+    <t>ML implementation</t>
+  </si>
+  <si>
+    <t>FS/EM Implementation</t>
+  </si>
+  <si>
+    <t>AHL (2019)</t>
+  </si>
+  <si>
+    <t>Lahiri &amp; Larsen (2005)</t>
+  </si>
+  <si>
+    <t>Goldstein et al. (2012)</t>
+  </si>
+  <si>
+    <t>Nix &amp; Qian (2015)</t>
+  </si>
+  <si>
+    <t>Bleakley &amp; Ferrie (2016)</t>
+  </si>
+  <si>
+    <t>Anderson (2019)</t>
   </si>
 </sst>
 </file>
@@ -311,10 +360,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -598,8 +650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="M57" sqref="M55:M57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -912,4 +964,89 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" customWidth="1"/>
+    <col min="4" max="4" width="23.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>